<commit_message>
zooplankton parser is creating local plankton samples
</commit_message>
<xml_diff>
--- a/core/tests/sample_data/sample_zoo.xlsx
+++ b/core/tests/sample_data/sample_zoo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DFO-MPO\Tallywacker Current\HL_02\HUD2021_185\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gov\Projects\djangoProject\dart2\core\tests\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F532833-8202-4AEE-829D-1CB600F6E874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF75F2-E1D3-4511-9FD9-2809953DC09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8117AA55-9F5E-4EFF-A7A2-67D717474FF6}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{8117AA55-9F5E-4EFF-A7A2-67D717474FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="65">
   <si>
     <t>MISSION</t>
   </si>
@@ -87,9 +87,6 @@
     <t>HUD2021_185</t>
   </si>
   <si>
-    <t>Sep 16/21</t>
-  </si>
-  <si>
     <t>HL_02</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>Pseudocalanus</t>
-  </si>
-  <si>
-    <t>Sep 22/21</t>
   </si>
   <si>
     <t>34-1</t>
@@ -276,10 +270,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,37 +592,37 @@
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H33"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -658,19 +653,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>13</v>
@@ -686,14 +681,14 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
+      <c r="B2" s="3">
+        <v>44455</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1">
         <v>202</v>
@@ -720,7 +715,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N2" s="1">
         <v>58</v>
@@ -745,14 +740,14 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
+      <c r="B3" s="3">
+        <v>44456</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
         <v>202</v>
@@ -779,7 +774,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N3" s="1">
         <v>58</v>
@@ -801,14 +796,14 @@
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
+      <c r="B4" s="3">
+        <v>44457</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>202</v>
@@ -835,7 +830,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N4" s="1">
         <v>58</v>
@@ -857,14 +852,14 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
+      <c r="B5" s="3">
+        <v>44458</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
         <v>202</v>
@@ -891,7 +886,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N5" s="1">
         <v>74</v>
@@ -913,14 +908,14 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
+      <c r="B6" s="3">
+        <v>44459</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1">
         <v>202</v>
@@ -947,7 +942,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6" s="1">
         <v>93</v>
@@ -966,14 +961,14 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
+      <c r="B7" s="3">
+        <v>44460</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1">
         <v>202</v>
@@ -1000,7 +995,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N7" s="1">
         <v>92</v>
@@ -1019,14 +1014,14 @@
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
+      <c r="B8" s="3">
+        <v>44461</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1">
         <v>202</v>
@@ -1053,7 +1048,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N8" s="1">
         <v>96</v>
@@ -1072,14 +1067,14 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
+      <c r="B9" s="3">
+        <v>44462</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1">
         <v>202</v>
@@ -1106,7 +1101,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N9" s="1">
         <v>150</v>
@@ -1128,14 +1123,14 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
+      <c r="B10" s="3">
+        <v>44463</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1">
         <v>202</v>
@@ -1162,7 +1157,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N10" s="1">
         <v>180</v>
@@ -1184,14 +1179,14 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
+      <c r="B11" s="3">
+        <v>44464</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1">
         <v>202</v>
@@ -1218,7 +1213,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N11" s="1">
         <v>119</v>
@@ -1237,14 +1232,14 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
+      <c r="B12" s="3">
+        <v>44465</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1">
         <v>202</v>
@@ -1271,7 +1266,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N12" s="1">
         <v>68</v>
@@ -1290,14 +1285,14 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
+      <c r="B13" s="3">
+        <v>44466</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1">
         <v>202</v>
@@ -1324,7 +1319,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N13" s="1">
         <v>67</v>
@@ -1343,14 +1338,14 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
+      <c r="B14" s="3">
+        <v>44467</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1">
         <v>202</v>
@@ -1377,7 +1372,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N14" s="1">
         <v>121</v>
@@ -1396,14 +1391,14 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
+      <c r="B15" s="3">
+        <v>44468</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1">
         <v>202</v>
@@ -1430,7 +1425,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N15" s="1">
         <v>683</v>
@@ -1449,14 +1444,14 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
+      <c r="B16" s="3">
+        <v>44469</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1">
         <v>202</v>
@@ -1483,7 +1478,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N16" s="1">
         <v>128</v>
@@ -1502,14 +1497,14 @@
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
+      <c r="B17" s="3">
+        <v>44470</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1">
         <v>202</v>
@@ -1536,7 +1531,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N17" s="1">
         <v>125</v>
@@ -1555,14 +1550,14 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
+      <c r="B18" s="3">
+        <v>44471</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1">
         <v>202</v>
@@ -1589,7 +1584,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N18" s="1">
         <v>127</v>
@@ -1608,14 +1603,14 @@
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
+      <c r="B19" s="3">
+        <v>44472</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="1">
         <v>202</v>
@@ -1642,7 +1637,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="1">
         <v>134</v>
@@ -1661,14 +1656,14 @@
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
+      <c r="B20" s="3">
+        <v>44473</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1">
         <v>202</v>
@@ -1695,7 +1690,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N20" s="1">
         <v>138</v>
@@ -1714,14 +1709,14 @@
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
+      <c r="B21" s="3">
+        <v>44474</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1">
         <v>202</v>
@@ -1748,7 +1743,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N21" s="1">
         <v>9</v>
@@ -1767,14 +1762,14 @@
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
+      <c r="B22" s="3">
+        <v>44475</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1">
         <v>202</v>
@@ -1801,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N22" s="1">
         <v>420</v>
@@ -1820,14 +1815,14 @@
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
+      <c r="B23" s="3">
+        <v>44476</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" s="1">
         <v>202</v>
@@ -1854,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N23" s="1">
         <v>693</v>
@@ -1873,14 +1868,14 @@
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
+      <c r="B24" s="3">
+        <v>44477</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1">
         <v>202</v>
@@ -1907,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N24" s="1">
         <v>2445</v>
@@ -1926,14 +1921,14 @@
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>17</v>
+      <c r="B25" s="3">
+        <v>44478</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" s="1">
         <v>202</v>
@@ -1960,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N25" s="1">
         <v>424</v>
@@ -1979,14 +1974,14 @@
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>17</v>
+      <c r="B26" s="3">
+        <v>44479</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" s="1">
         <v>202</v>
@@ -2013,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N26" s="1">
         <v>1608</v>
@@ -2032,14 +2027,14 @@
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>17</v>
+      <c r="B27" s="3">
+        <v>44480</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E27" s="1">
         <v>202</v>
@@ -2066,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N27" s="1">
         <v>420</v>
@@ -2085,14 +2080,14 @@
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>17</v>
+      <c r="B28" s="3">
+        <v>44481</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28" s="1">
         <v>202</v>
@@ -2119,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N28" s="1">
         <v>693</v>
@@ -2138,14 +2133,14 @@
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>17</v>
+      <c r="B29" s="3">
+        <v>44482</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1">
         <v>202</v>
@@ -2172,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N29" s="1">
         <v>2445</v>
@@ -2191,14 +2186,14 @@
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>17</v>
+      <c r="B30" s="3">
+        <v>44483</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1">
         <v>202</v>
@@ -2225,7 +2220,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N30" s="1">
         <v>424</v>
@@ -2244,14 +2239,14 @@
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>17</v>
+      <c r="B31" s="3">
+        <v>44484</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1">
         <v>202</v>
@@ -2278,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N31" s="1">
         <v>1608</v>
@@ -2297,14 +2292,14 @@
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>17</v>
+      <c r="B32" s="3">
+        <v>44485</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E32" s="1">
         <v>202</v>
@@ -2331,7 +2326,7 @@
         <v>1</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N32" s="1">
         <v>1608</v>
@@ -2350,14 +2345,14 @@
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>17</v>
+      <c r="B33" s="3">
+        <v>44486</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E33" s="1">
         <v>202</v>
@@ -2384,7 +2379,7 @@
         <v>0.5</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N33" s="1">
         <v>1608</v>
@@ -2403,14 +2398,14 @@
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>37</v>
+      <c r="B34" s="3">
+        <v>44487</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E34" s="1">
         <v>202</v>
@@ -2437,7 +2432,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N34" s="1">
         <v>17</v>
@@ -2459,14 +2454,14 @@
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
+      <c r="B35" s="3">
+        <v>44488</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E35" s="1">
         <v>202</v>
@@ -2493,7 +2488,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N35" s="1">
         <v>210</v>
@@ -2515,14 +2510,14 @@
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>37</v>
+      <c r="B36" s="3">
+        <v>44489</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E36" s="1">
         <v>202</v>
@@ -2549,7 +2544,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N36" s="1">
         <v>39</v>
@@ -2571,14 +2566,14 @@
       <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>37</v>
+      <c r="B37" s="3">
+        <v>44490</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E37" s="1">
         <v>202</v>
@@ -2605,7 +2600,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N37" s="1">
         <v>58</v>
@@ -2630,14 +2625,14 @@
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>37</v>
+      <c r="B38" s="3">
+        <v>44491</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="1">
         <v>202</v>
@@ -2664,7 +2659,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N38" s="1">
         <v>58</v>
@@ -2686,14 +2681,14 @@
       <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>37</v>
+      <c r="B39" s="3">
+        <v>44492</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E39" s="1">
         <v>202</v>
@@ -2720,7 +2715,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N39" s="1">
         <v>58</v>
@@ -2742,14 +2737,14 @@
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
+      <c r="B40" s="3">
+        <v>44493</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E40" s="1">
         <v>202</v>
@@ -2776,7 +2771,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N40" s="1">
         <v>58</v>
@@ -2798,14 +2793,14 @@
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>37</v>
+      <c r="B41" s="3">
+        <v>44494</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E41" s="1">
         <v>202</v>
@@ -2832,7 +2827,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N41" s="1">
         <v>74</v>
@@ -2854,14 +2849,14 @@
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>37</v>
+      <c r="B42" s="3">
+        <v>44495</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E42" s="1">
         <v>202</v>
@@ -2888,7 +2883,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N42" s="1">
         <v>74</v>
@@ -2910,14 +2905,14 @@
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>37</v>
+      <c r="B43" s="3">
+        <v>44496</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E43" s="1">
         <v>202</v>
@@ -2944,7 +2939,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N43" s="1">
         <v>93</v>
@@ -2963,14 +2958,14 @@
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>37</v>
+      <c r="B44" s="3">
+        <v>44497</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E44" s="1">
         <v>202</v>
@@ -2997,7 +2992,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N44" s="1">
         <v>92</v>
@@ -3016,14 +3011,14 @@
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>37</v>
+      <c r="B45" s="3">
+        <v>44498</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E45" s="1">
         <v>202</v>
@@ -3050,7 +3045,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N45" s="1">
         <v>96</v>
@@ -3069,14 +3064,14 @@
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>37</v>
+      <c r="B46" s="3">
+        <v>44499</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E46" s="1">
         <v>202</v>
@@ -3103,7 +3098,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N46" s="1">
         <v>150</v>
@@ -3125,14 +3120,14 @@
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>37</v>
+      <c r="B47" s="3">
+        <v>44500</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E47" s="1">
         <v>202</v>
@@ -3159,7 +3154,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N47" s="1">
         <v>250</v>
@@ -3181,14 +3176,14 @@
       <c r="A48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>37</v>
+      <c r="B48" s="3">
+        <v>44501</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E48" s="1">
         <v>202</v>
@@ -3215,7 +3210,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N48" s="1">
         <v>180</v>
@@ -3237,14 +3232,14 @@
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>37</v>
+      <c r="B49" s="3">
+        <v>44502</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E49" s="1">
         <v>202</v>
@@ -3271,7 +3266,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N49" s="1">
         <v>180</v>
@@ -3293,14 +3288,14 @@
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>37</v>
+      <c r="B50" s="3">
+        <v>44503</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E50" s="1">
         <v>202</v>
@@ -3327,7 +3322,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N50" s="1">
         <v>180</v>
@@ -3349,14 +3344,14 @@
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>37</v>
+      <c r="B51" s="3">
+        <v>44504</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E51" s="1">
         <v>202</v>
@@ -3383,7 +3378,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N51" s="1">
         <v>31</v>
@@ -3402,14 +3397,14 @@
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>37</v>
+      <c r="B52" s="3">
+        <v>44505</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E52" s="1">
         <v>202</v>
@@ -3436,7 +3431,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N52" s="1">
         <v>206</v>
@@ -3455,14 +3450,14 @@
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>37</v>
+      <c r="B53" s="3">
+        <v>44506</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E53" s="1">
         <v>202</v>
@@ -3489,7 +3484,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N53" s="1">
         <v>271</v>
@@ -3508,14 +3503,14 @@
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>37</v>
+      <c r="B54" s="3">
+        <v>44507</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E54" s="1">
         <v>202</v>
@@ -3542,7 +3537,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N54" s="1">
         <v>226</v>
@@ -3561,14 +3556,14 @@
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>37</v>
+      <c r="B55" s="3">
+        <v>44508</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E55" s="1">
         <v>202</v>
@@ -3595,7 +3590,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N55" s="1">
         <v>222</v>
@@ -3614,14 +3609,14 @@
       <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>37</v>
+      <c r="B56" s="3">
+        <v>44509</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E56" s="1">
         <v>202</v>
@@ -3648,7 +3643,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N56" s="1">
         <v>119</v>
@@ -3667,14 +3662,14 @@
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>37</v>
+      <c r="B57" s="3">
+        <v>44510</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E57" s="1">
         <v>202</v>
@@ -3701,7 +3696,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N57" s="1">
         <v>68</v>
@@ -3720,14 +3715,14 @@
       <c r="A58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>37</v>
+      <c r="B58" s="3">
+        <v>44511</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E58" s="1">
         <v>202</v>
@@ -3754,7 +3749,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N58" s="1">
         <v>67</v>
@@ -3773,14 +3768,14 @@
       <c r="A59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>37</v>
+      <c r="B59" s="3">
+        <v>44512</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E59" s="1">
         <v>202</v>
@@ -3807,7 +3802,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N59" s="1">
         <v>121</v>
@@ -3826,14 +3821,14 @@
       <c r="A60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>37</v>
+      <c r="B60" s="3">
+        <v>44513</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E60" s="1">
         <v>202</v>
@@ -3860,7 +3855,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N60" s="1">
         <v>683</v>
@@ -3879,14 +3874,14 @@
       <c r="A61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>37</v>
+      <c r="B61" s="3">
+        <v>44514</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E61" s="1">
         <v>202</v>
@@ -3913,7 +3908,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N61" s="1">
         <v>128</v>
@@ -3932,14 +3927,14 @@
       <c r="A62" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>37</v>
+      <c r="B62" s="3">
+        <v>44515</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E62" s="1">
         <v>202</v>
@@ -3966,7 +3961,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N62" s="1">
         <v>127</v>
@@ -3985,14 +3980,14 @@
       <c r="A63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>37</v>
+      <c r="B63" s="3">
+        <v>44516</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E63" s="1">
         <v>202</v>
@@ -4019,7 +4014,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N63" s="1">
         <v>134</v>
@@ -4038,14 +4033,14 @@
       <c r="A64" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>37</v>
+      <c r="B64" s="3">
+        <v>44517</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E64" s="1">
         <v>202</v>
@@ -4072,7 +4067,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N64" s="1">
         <v>33</v>
@@ -4091,14 +4086,14 @@
       <c r="A65" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>37</v>
+      <c r="B65" s="3">
+        <v>44518</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E65" s="1">
         <v>202</v>
@@ -4125,7 +4120,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N65" s="1">
         <v>138</v>
@@ -4144,14 +4139,14 @@
       <c r="A66" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>37</v>
+      <c r="B66" s="3">
+        <v>44519</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E66" s="1">
         <v>202</v>
@@ -4178,7 +4173,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N66" s="1">
         <v>9</v>
@@ -4197,14 +4192,14 @@
       <c r="A67" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>37</v>
+      <c r="B67" s="3">
+        <v>44520</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E67" s="1">
         <v>202</v>
@@ -4231,7 +4226,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N67" s="1">
         <v>522</v>
@@ -4250,14 +4245,14 @@
       <c r="A68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>37</v>
+      <c r="B68" s="3">
+        <v>44521</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E68" s="1">
         <v>202</v>
@@ -4284,7 +4279,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N68" s="1">
         <v>147</v>
@@ -4303,14 +4298,14 @@
       <c r="A69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>37</v>
+      <c r="B69" s="3">
+        <v>44522</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E69" s="1">
         <v>202</v>
@@ -4337,7 +4332,7 @@
         <v>1</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N69" s="1">
         <v>3657</v>
@@ -4356,14 +4351,14 @@
       <c r="A70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>37</v>
+      <c r="B70" s="3">
+        <v>44523</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E70" s="1">
         <v>202</v>
@@ -4390,7 +4385,7 @@
         <v>1</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N70" s="1">
         <v>5506</v>
@@ -4409,14 +4404,14 @@
       <c r="A71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>37</v>
+      <c r="B71" s="3">
+        <v>44524</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E71" s="1">
         <v>202</v>
@@ -4443,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N71" s="1">
         <v>693</v>
@@ -4462,14 +4457,14 @@
       <c r="A72" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>37</v>
+      <c r="B72" s="3">
+        <v>44525</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E72" s="1">
         <v>202</v>
@@ -4496,7 +4491,7 @@
         <v>1</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N72" s="1">
         <v>1608</v>
@@ -4515,14 +4510,14 @@
       <c r="A73" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>37</v>
+      <c r="B73" s="3">
+        <v>44526</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E73" s="1">
         <v>202</v>
@@ -4549,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N73" s="1">
         <v>3657</v>
@@ -4568,14 +4563,14 @@
       <c r="A74" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>37</v>
+      <c r="B74" s="3">
+        <v>44527</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E74" s="1">
         <v>202</v>
@@ -4602,7 +4597,7 @@
         <v>1</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N74" s="1">
         <v>5506</v>
@@ -4621,14 +4616,14 @@
       <c r="A75" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>37</v>
+      <c r="B75" s="3">
+        <v>44528</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E75" s="1">
         <v>202</v>
@@ -4655,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N75" s="1">
         <v>693</v>
@@ -4674,14 +4669,14 @@
       <c r="A76" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>37</v>
+      <c r="B76" s="3">
+        <v>44529</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E76" s="1">
         <v>202</v>
@@ -4708,7 +4703,7 @@
         <v>1</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N76" s="1">
         <v>1608</v>
@@ -4727,14 +4722,14 @@
       <c r="A77" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>37</v>
+      <c r="B77" s="3">
+        <v>44530</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E77" s="1">
         <v>202</v>
@@ -4761,7 +4756,7 @@
         <v>1</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N77" s="1">
         <v>1608</v>
@@ -4780,14 +4775,14 @@
       <c r="A78" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>37</v>
+      <c r="B78" s="3">
+        <v>44531</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E78" s="1">
         <v>202</v>
@@ -4814,7 +4809,7 @@
         <v>0.5</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N78" s="1">
         <v>1608</v>

</xml_diff>